<commit_message>
Updated the Item Categories in Output Files
1. Update the Item categories in output files.
2. Corrected the calculation of food at home tax rates.
</commit_message>
<xml_diff>
--- a/input/cu-all-multi-year-2006-2012_new_Jiaxi.xlsx
+++ b/input/cu-all-multi-year-2006-2012_new_Jiaxi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiaxitan/UMN/Fed RA/Heathcote/sales_taxes/main/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D802B2CF-265C-0549-B6AB-F447FB5890B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C568ADC4-2C1C-B649-A927-3B6B60BB5B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43920" yWindow="1420" windowWidth="34880" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32900" yWindow="3380" windowWidth="39780" windowHeight="23940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -1208,9 +1208,9 @@
   </sheetPr>
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B113" sqref="B113"/>
+      <selection pane="topRight" activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3114,7 +3114,7 @@
         <v>3.8611280124533614E-3</v>
       </c>
       <c r="F90" s="64">
-        <f t="shared" ref="F90:F93" si="4">C90/$D$89</f>
+        <f>C90/$D$89</f>
         <v>7.8435214922069202E-2</v>
       </c>
       <c r="G90" s="84"/>
@@ -3122,7 +3122,7 @@
         <v>243</v>
       </c>
       <c r="I90" s="40">
-        <f t="shared" ref="I90:I95" si="5">H90/H$7</f>
+        <f t="shared" ref="I90:I95" si="4">H90/H$7</f>
         <v>5.0510299528154813E-3</v>
       </c>
       <c r="J90" s="9"/>
@@ -3141,7 +3141,7 @@
         <v>1.4948071097347087E-2</v>
       </c>
       <c r="F91" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F90:F93" si="5">C91/$D$89</f>
         <v>0.30365612468927472</v>
       </c>
       <c r="G91" s="84"/>
@@ -3149,7 +3149,7 @@
         <v>787</v>
       </c>
       <c r="I91" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.6358685485044377E-2</v>
       </c>
       <c r="J91" s="5">
@@ -3170,7 +3170,7 @@
         <v>1.9267411072044497E-2</v>
       </c>
       <c r="F92" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.39139948832398885</v>
       </c>
       <c r="G92" s="84"/>
@@ -3178,7 +3178,7 @@
         <v>1010</v>
       </c>
       <c r="I92" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.0993992807998504E-2</v>
       </c>
       <c r="J92" s="5"/>
@@ -3199,7 +3199,7 @@
         <v>1.1150181694887641E-2</v>
       </c>
       <c r="F93" s="64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.22650554315678695</v>
       </c>
       <c r="G93" s="84"/>
@@ -3207,7 +3207,7 @@
         <v>423</v>
       </c>
       <c r="I93" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.7925336215676896E-3</v>
       </c>
       <c r="J93" s="5">
@@ -3235,7 +3235,7 @@
         <v>493</v>
       </c>
       <c r="I94" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.0247562826082439E-2</v>
       </c>
       <c r="J94" s="5">
@@ -3261,7 +3261,7 @@
         <v>3157</v>
       </c>
       <c r="I95" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.5621817123615117E-2</v>
       </c>
       <c r="J95" s="5"/>
@@ -3341,7 +3341,9 @@
       </c>
       <c r="E100" s="63"/>
       <c r="F100" s="63"/>
-      <c r="G100" s="83"/>
+      <c r="G100" s="83">
+        <v>4</v>
+      </c>
       <c r="H100" s="5">
         <v>2504</v>
       </c>
@@ -3361,7 +3363,10 @@
         <f>C101/D$7</f>
         <v>1.1651088650884645E-2</v>
       </c>
-      <c r="F101" s="64"/>
+      <c r="F101" s="64">
+        <f>C101/$D$100</f>
+        <v>0.22948414359955949</v>
+      </c>
       <c r="G101" s="84"/>
       <c r="H101" s="9">
         <v>581</v>
@@ -3387,7 +3392,10 @@
         <f>C102/D$7</f>
         <v>1.9357624343363498E-2</v>
       </c>
-      <c r="F102" s="64"/>
+      <c r="F102" s="64">
+        <f t="shared" ref="F102:F104" si="6">C102/$D$100</f>
+        <v>0.3812749158183999</v>
+      </c>
       <c r="G102" s="84"/>
       <c r="H102" s="9">
         <v>954</v>
@@ -3413,7 +3421,10 @@
         <f>C103/D$7</f>
         <v>1.1667344903736188E-2</v>
       </c>
-      <c r="F103" s="64"/>
+      <c r="F103" s="64">
+        <f t="shared" si="6"/>
+        <v>0.22980433275746198</v>
+      </c>
       <c r="G103" s="84"/>
       <c r="H103" s="9">
         <v>606</v>
@@ -3439,7 +3450,10 @@
         <f>C104/D$7</f>
         <v>8.0947207193624113E-3</v>
       </c>
-      <c r="F104" s="64"/>
+      <c r="F104" s="64">
+        <f t="shared" si="6"/>
+        <v>0.15943660782457855</v>
+      </c>
       <c r="G104" s="84"/>
       <c r="H104" s="9">
         <v>364</v>
@@ -3660,7 +3674,7 @@
         <v>1.2442285836373492E-3</v>
       </c>
       <c r="F113" s="64">
-        <f t="shared" ref="F113:F115" si="6">C113/$D$111</f>
+        <f t="shared" ref="F113:F115" si="7">C113/$D$111</f>
         <v>7.9964638752712369E-2</v>
       </c>
       <c r="G113" s="84"/>
@@ -3684,7 +3698,7 @@
         <v>1.1223960073213875E-3</v>
       </c>
       <c r="F114" s="64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.2134648281879654E-2</v>
       </c>
       <c r="G114" s="84"/>
@@ -3709,7 +3723,7 @@
         <v>1.0422759039816385E-2</v>
       </c>
       <c r="F115" s="64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.669854536687294</v>
       </c>
       <c r="G115" s="84"/>

</xml_diff>

<commit_message>
(1) Re-organized folders; (2) Corrected JF code for utilities
</commit_message>
<xml_diff>
--- a/input/cu-all-multi-year-2006-2012_new_Jiaxi.xlsx
+++ b/input/cu-all-multi-year-2006-2012_new_Jiaxi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiaxitan/UMN/Fed RA/Heathcote/sales_taxes/main/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C568ADC4-2C1C-B649-A927-3B6B60BB5B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BF939D-C62D-1B4E-AF9B-9DCE8A97D1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32900" yWindow="3380" windowWidth="39780" windowHeight="23940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="11640" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -364,21 +364,6 @@
     <t>Not Taxed</t>
   </si>
   <si>
-    <t>JF 34</t>
-  </si>
-  <si>
-    <t>JF 32</t>
-  </si>
-  <si>
-    <t>JF 35</t>
-  </si>
-  <si>
-    <t>JF 30</t>
-  </si>
-  <si>
-    <t>JF 33</t>
-  </si>
-  <si>
     <t>Taxable in some states, at reduced rates (from Book of States Table 7.11 for 2010)</t>
   </si>
   <si>
@@ -497,6 +482,21 @@
   </si>
   <si>
     <t>2015_sub</t>
+  </si>
+  <si>
+    <t>JF 42</t>
+  </si>
+  <si>
+    <t>JF 40</t>
+  </si>
+  <si>
+    <t>JF 43</t>
+  </si>
+  <si>
+    <t>JF 38</t>
+  </si>
+  <si>
+    <t>JF 41</t>
   </si>
 </sst>
 </file>
@@ -1208,9 +1208,9 @@
   </sheetPr>
   <dimension ref="A1:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G102" sqref="G102"/>
+      <selection pane="topRight" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1228,7 +1228,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="66" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1251,31 +1251,31 @@
         <v>0</v>
       </c>
       <c r="B3" s="87" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D3" s="1">
         <v>2015</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H3" s="1">
         <v>2010</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="B8" s="69"/>
       <c r="C8" s="54" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D8" s="46">
         <f>D10+D35+D36+D40+D41+C43+C44+D45+C47+C48+C49+C51+C52+C53+C54+C55+C57+C58+C59+D60+D64+D72+D84+D88+C90+C91+C92+C93+D94+D95+C101+C102+C103+C104+C106+C107+D108+D109+D110+C112+C113+C114+C115+D117+D119</f>
@@ -1378,7 +1378,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C10" s="55"/>
       <c r="D10" s="47">
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="4" customFormat="1" ht="12.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -1898,7 +1898,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="72" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="51">
@@ -2049,7 +2049,7 @@
     <row r="43" spans="1:13" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="27"/>
       <c r="B43" s="75" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C43" s="49">
         <f>D42-C44</f>
@@ -2076,7 +2076,7 @@
     <row r="44" spans="1:13" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="18"/>
       <c r="B44" s="73" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C44" s="57">
         <v>418.12</v>
@@ -2151,7 +2151,7 @@
     <row r="47" spans="1:13" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="26"/>
       <c r="B47" s="75" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C47" s="49">
         <v>415.76</v>
@@ -2177,7 +2177,7 @@
     <row r="48" spans="1:13" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="26"/>
       <c r="B48" s="75" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C48" s="49">
         <v>71.12</v>
@@ -2203,7 +2203,7 @@
     <row r="49" spans="1:13" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="20"/>
       <c r="B49" s="73" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C49" s="57">
         <f>D46-C47-C48</f>
@@ -2230,7 +2230,7 @@
         <v>39</v>
       </c>
       <c r="B50" s="77" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C50" s="39"/>
       <c r="D50" s="46">
@@ -2254,7 +2254,7 @@
         <v>40</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="C51" s="49">
         <v>421.29</v>
@@ -2287,7 +2287,7 @@
         <v>41</v>
       </c>
       <c r="B52" s="75" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="C52" s="49">
         <v>1459.98</v>
@@ -2320,7 +2320,7 @@
         <v>42</v>
       </c>
       <c r="B53" s="75" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="C53" s="49">
         <v>116.35</v>
@@ -2353,7 +2353,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="75" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="C54" s="49">
         <v>1347.12</v>
@@ -2386,7 +2386,7 @@
         <v>44</v>
       </c>
       <c r="B55" s="75" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="C55" s="49">
         <v>540.37</v>
@@ -2441,7 +2441,7 @@
         <v>46</v>
       </c>
       <c r="B57" s="72" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C57" s="57">
         <v>426.78</v>
@@ -2472,7 +2472,7 @@
         <v>47</v>
       </c>
       <c r="B58" s="72" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C58" s="57">
         <f>D56-C57-C59</f>
@@ -2502,7 +2502,7 @@
     <row r="59" spans="1:13" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="26"/>
       <c r="B59" s="70" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C59" s="49">
         <f>413.14</f>
@@ -3059,7 +3059,7 @@
         <v>74</v>
       </c>
       <c r="B88" s="72" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C88" s="57"/>
       <c r="D88" s="51">
@@ -3141,7 +3141,7 @@
         <v>1.4948071097347087E-2</v>
       </c>
       <c r="F91" s="64">
-        <f t="shared" ref="F90:F93" si="5">C91/$D$89</f>
+        <f t="shared" ref="F91:F93" si="5">C91/$D$89</f>
         <v>0.30365612468927472</v>
       </c>
       <c r="G91" s="84"/>
@@ -3188,7 +3188,7 @@
         <v>79</v>
       </c>
       <c r="B93" s="75" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C93" s="49">
         <v>624.16999999999996</v>
@@ -3219,7 +3219,7 @@
         <v>80</v>
       </c>
       <c r="B94" s="75" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C94" s="49"/>
       <c r="D94" s="47">
@@ -3485,7 +3485,7 @@
     <row r="106" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="22"/>
       <c r="B106" s="75" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C106" s="49">
         <v>309.02</v>
@@ -3514,7 +3514,7 @@
     <row r="107" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="16"/>
       <c r="B107" s="71" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C107" s="56">
         <v>373.54</v>
@@ -3590,7 +3590,7 @@
         <v>94</v>
       </c>
       <c r="B110" s="72" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C110" s="57"/>
       <c r="D110" s="51">
@@ -3616,7 +3616,7 @@
         <v>95</v>
       </c>
       <c r="B111" s="78" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C111" s="58"/>
       <c r="D111" s="52">
@@ -3639,7 +3639,7 @@
     <row r="112" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="22"/>
       <c r="B112" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C112" s="49">
         <v>155.08000000000001</v>
@@ -3663,7 +3663,7 @@
     <row r="113" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="22"/>
       <c r="B113" s="70" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C113" s="49">
         <v>69.650000000000006</v>
@@ -3687,7 +3687,7 @@
     <row r="114" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="22"/>
       <c r="B114" s="70" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C114" s="49">
         <v>62.83</v>
@@ -3711,7 +3711,7 @@
     <row r="115" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="15"/>
       <c r="B115" s="72" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C115" s="57">
         <f>D111-C112-C113-C114</f>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="122" spans="1:10" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B122" s="59"/>
       <c r="C122" s="54"/>
@@ -3853,7 +3853,7 @@
       <c r="F122" s="43"/>
       <c r="G122" s="85"/>
       <c r="H122" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I122" s="43">
         <f>SUM(I10:I121)</f>
@@ -3967,16 +3967,16 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="C3" s="33" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
@@ -4102,12 +4102,12 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="33" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>